<commit_message>
fixed missing co2 compression electricity connection
</commit_message>
<xml_diff>
--- a/data/steel/factories/DRI_factory-HC.xlsx
+++ b/data/steel/factories/DRI_factory-HC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/steel/factories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B5AD0F-C1EF-5B48-B18C-8118A96E52E5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64EBA1EC-6FDA-5741-9162-6C8C3DC9E1AC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20360" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3380" yWindow="460" windowWidth="20360" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="chains" sheetId="9" r:id="rId1"/>
@@ -818,7 +818,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1508,7 +1508,7 @@
         <v>48</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D25" t="s">
         <v>5</v>
@@ -1617,7 +1617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2594CE52-C30C-EE4C-A797-A397203AD571}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
removed waste heat recovery
from electricity to co2 capture. Now no waste heat is considered at all.
</commit_message>
<xml_diff>
--- a/data/steel/factories/DRI_factory-HC.xlsx
+++ b/data/steel/factories/DRI_factory-HC.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/steel/factories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\BlackBlox\data\steel\factories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64EBA1EC-6FDA-5741-9162-6C8C3DC9E1AC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3380" yWindow="460" windowWidth="20360" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3375" yWindow="465" windowWidth="20355" windowHeight="17535" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="chains" sheetId="9" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="steel" sheetId="2" r:id="rId3"/>
     <sheet name="CO2" sheetId="10" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="68">
   <si>
     <t>Inflow</t>
   </si>
@@ -207,12 +206,6 @@
     <t>steel scrap</t>
   </si>
   <si>
-    <t>waste heat</t>
-  </si>
-  <si>
-    <t>recovered heat</t>
-  </si>
-  <si>
     <t>heat</t>
   </si>
   <si>
@@ -241,9 +234,6 @@
   </si>
   <si>
     <t>aux CO2 cap</t>
-  </si>
-  <si>
-    <t>heat recovery</t>
   </si>
   <si>
     <t>CO2 storage</t>
@@ -252,7 +242,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -339,7 +329,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -650,21 +640,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -681,7 +671,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -695,7 +685,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -709,7 +699,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -723,7 +713,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -737,7 +727,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -751,7 +741,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -765,9 +755,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
         <v>46</v>
@@ -776,24 +766,24 @@
         <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -814,30 +804,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+    <col min="1" max="1" width="11.375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.875" customWidth="1"/>
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -875,7 +865,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -907,7 +897,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -933,7 +923,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -959,7 +949,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -985,7 +975,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>40</v>
       </c>
@@ -1014,9 +1004,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1043,7 +1033,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -1069,7 +1059,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>19</v>
       </c>
@@ -1095,7 +1085,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>40</v>
       </c>
@@ -1121,9 +1111,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -1150,7 +1140,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>40</v>
       </c>
@@ -1176,7 +1166,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>45</v>
       </c>
@@ -1202,41 +1192,41 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>68</v>
-      </c>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="G14" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="B15" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1251,18 +1241,18 @@
         <v>53</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s">
         <v>17</v>
@@ -1277,100 +1267,94 @@
         <v>53</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" t="s">
         <v>5</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F18" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G17" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="1" t="s">
+      <c r="G18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" t="s">
-        <v>57</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G18" t="s">
-        <v>53</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I18" t="s">
-        <v>45</v>
-      </c>
-      <c r="J18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E19" t="s">
         <v>57</v>
       </c>
       <c r="F19" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" t="s">
         <v>58</v>
       </c>
-      <c r="G19" t="s">
-        <v>53</v>
-      </c>
       <c r="H19" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I19" t="s">
-        <v>62</v>
-      </c>
-      <c r="J19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="B20" t="s">
         <v>45</v>
       </c>
@@ -1378,154 +1362,99 @@
         <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E20" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G21" t="s">
+        <v>53</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>60</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" t="s">
-        <v>59</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="G21" t="s">
-        <v>60</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" t="s">
-        <v>64</v>
-      </c>
       <c r="F22" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G22" t="s">
         <v>53</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I22" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" t="s">
-        <v>43</v>
+        <v>48</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="G23" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="I23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" t="s">
-        <v>64</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="G24" t="s">
-        <v>53</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" t="s">
-        <v>21</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G25" t="s">
-        <v>17</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I25" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1535,21 +1464,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="2" max="2" width="18.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1560,7 +1489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1571,7 +1500,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -1582,7 +1511,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>44</v>
       </c>
@@ -1593,7 +1522,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>31</v>
       </c>
@@ -1604,7 +1533,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
     </row>
@@ -1614,16 +1543,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2594CE52-C30C-EE4C-A797-A397203AD571}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1634,18 +1563,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>52</v>
       </c>

</xml_diff>